<commit_message>
Preparing batch tests on the server.
</commit_message>
<xml_diff>
--- a/results/2017-03-24 - lotOfois/Stats.xlsx
+++ b/results/2017-03-24 - lotOfois/Stats.xlsx
@@ -4,21 +4,42 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$T$80</definedName>
+    <definedName name="dadosBrutos___Copia" localSheetId="1">Sheet1!$A$1:$E$80</definedName>
     <definedName name="results_1" localSheetId="0">Sheet2!$A$1:$E$21</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="results1" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" name="dadosBrutos - Copia" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\bruno\Documents\_gits\surveillanceStrategies\results\2017-03-24 - lotOfois\dadosBrutos - Copia.txt" decimal="," thousands="." tab="0" semicolon="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="results1" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\bruno\Documents\_gits\surveillanceStrategies\results\2017-03-20 - lotOfPois\results.txt" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="12">
         <textField/>
@@ -40,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="6">
   <si>
     <t>Strategy</t>
   </si>
@@ -65,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,19 +549,189 @@
             <c:numRef>
               <c:f>Sheet2!$D$18:$D$21</c:f>
               <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.76884</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8503500000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8113499999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.487169999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$22:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$22:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$26:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$26:$D$29</c:f>
+              <c:numCache>
                 <c:formatCode>#.##00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.76884</c:v>
+                  <c:v>7.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8503500000000002</c:v>
+                  <c:v>14.86</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.8113499999999991</c:v>
+                  <c:v>41.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.487169999999999</c:v>
+                  <c:v>80.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,11 +746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="299802344"/>
-        <c:axId val="299805872"/>
+        <c:axId val="137361120"/>
+        <c:axId val="137364256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="299802344"/>
+        <c:axId val="137361120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,12 +804,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299805872"/>
+        <c:crossAx val="137364256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="299805872"/>
+        <c:axId val="137364256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -671,7 +863,721 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299802344"/>
+        <c:crossAx val="137361120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.8758599999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0227449999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.322600000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.341380000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.34477</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.07315</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.965450000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.704219999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$10:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$10:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.06223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5850799999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.781585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.663274999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$14:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$14:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.5187200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8488499999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.059519999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.208545000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$18:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$18:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.76884</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8503500000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8113499999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.487169999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$22:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$22:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="364319792"/>
+        <c:axId val="364320968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="364319792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364320968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="364320968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364319792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -788,6 +1694,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1304,6 +2250,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1311,13 +2773,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>33057</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>61632</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1336,11 +2798,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dadosBrutos - Copia" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1630,10 +3128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,6 +3500,163 @@
         <v>453</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>200</v>
+      </c>
+      <c r="D23" s="1">
+        <v>9.0500000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24" s="1">
+        <v>26.13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25" s="1">
+        <v>56.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>500</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>500</v>
+      </c>
+      <c r="D27" s="1">
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>125</v>
+      </c>
+      <c r="C28">
+        <v>500</v>
+      </c>
+      <c r="D28" s="1">
+        <v>41.86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>250</v>
+      </c>
+      <c r="C29">
+        <v>500</v>
+      </c>
+      <c r="D29" s="1">
+        <v>80.56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E21">
     <sortCondition descending="1" ref="C2"/>
@@ -2009,4 +3664,1406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:D77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.25255080000000002</v>
+      </c>
+      <c r="E2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4.6486099999999995E-2</v>
+      </c>
+      <c r="E3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9.1161100000000009E-2</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.55948189999999998</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.2330518</v>
+      </c>
+      <c r="E6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.6278899999999998E-2</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8.3835099999999996E-2</v>
+      </c>
+      <c r="E8">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.59889159999999997</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.29032550000000001</v>
+      </c>
+      <c r="E10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4.5178900000000001E-2</v>
+      </c>
+      <c r="E11">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7.89213E-2</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.52820770000000006</v>
+      </c>
+      <c r="E13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>200</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.2855567</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4.5157900000000001E-2</v>
+      </c>
+      <c r="E15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8.9184600000000003E-2</v>
+      </c>
+      <c r="E16">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>200</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.55223990000000001</v>
+      </c>
+      <c r="E17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.2232517</v>
+      </c>
+      <c r="E18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4.0672499999999993E-2</v>
+      </c>
+      <c r="E19">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8.5729299999999994E-2</v>
+      </c>
+      <c r="E20">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.57939590000000007</v>
+      </c>
+      <c r="E21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.297462</v>
+      </c>
+      <c r="E22">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>200</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4.6114499999999996E-2</v>
+      </c>
+      <c r="E23">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>200</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24" s="2">
+        <v>8.9286900000000002E-2</v>
+      </c>
+      <c r="E24">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>200</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.58521430000000008</v>
+      </c>
+      <c r="E25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>200</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.28001510000000002</v>
+      </c>
+      <c r="E26">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>200</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4.4462099999999997E-2</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>200</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.10562350000000001</v>
+      </c>
+      <c r="E28">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>200</v>
+      </c>
+      <c r="C29">
+        <v>100</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.57814489999999996</v>
+      </c>
+      <c r="E29">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>200</v>
+      </c>
+      <c r="C30">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.28897250000000002</v>
+      </c>
+      <c r="E30">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>200</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4.5869600000000003E-2</v>
+      </c>
+      <c r="E31">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>200</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32" s="2">
+        <v>9.5788600000000002E-2</v>
+      </c>
+      <c r="E32">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>200</v>
+      </c>
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.47666710000000001</v>
+      </c>
+      <c r="E33">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>200</v>
+      </c>
+      <c r="C34">
+        <v>50</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.22985720000000001</v>
+      </c>
+      <c r="E34">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>200</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" s="2">
+        <v>4.7041399999999997E-2</v>
+      </c>
+      <c r="E35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>200</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2">
+        <v>9.3564299999999989E-2</v>
+      </c>
+      <c r="E36">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>200</v>
+      </c>
+      <c r="C37">
+        <v>100</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.55976340000000002</v>
+      </c>
+      <c r="E37">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>200</v>
+      </c>
+      <c r="C38">
+        <v>50</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.23231089999999999</v>
+      </c>
+      <c r="E38">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>200</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4.5960400000000005E-2</v>
+      </c>
+      <c r="E39">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>200</v>
+      </c>
+      <c r="C40">
+        <v>20</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9.2128999999999989E-2</v>
+      </c>
+      <c r="E40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>200</v>
+      </c>
+      <c r="C41">
+        <v>100</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.59010969999999996</v>
+      </c>
+      <c r="E41">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>500</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42" s="2">
+        <v>7.4027999999999997E-2</v>
+      </c>
+      <c r="E42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>500</v>
+      </c>
+      <c r="C43">
+        <v>50</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.1449327</v>
+      </c>
+      <c r="E43">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>500</v>
+      </c>
+      <c r="C44">
+        <v>125</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.41484389999999999</v>
+      </c>
+      <c r="E44">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>500</v>
+      </c>
+      <c r="C45">
+        <v>250</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.82857439999999993</v>
+      </c>
+      <c r="E45">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>500</v>
+      </c>
+      <c r="C46">
+        <v>25</v>
+      </c>
+      <c r="D46" s="2">
+        <v>7.8381699999999999E-2</v>
+      </c>
+      <c r="E46">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>500</v>
+      </c>
+      <c r="C47">
+        <v>50</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.1486363</v>
+      </c>
+      <c r="E47">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>500</v>
+      </c>
+      <c r="C48">
+        <v>125</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.39702389999999999</v>
+      </c>
+      <c r="E48">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>500</v>
+      </c>
+      <c r="C49">
+        <v>250</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.80939710000000009</v>
+      </c>
+      <c r="E49">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>500</v>
+      </c>
+      <c r="C50">
+        <v>25</v>
+      </c>
+      <c r="D50" s="2">
+        <v>7.5831400000000007E-2</v>
+      </c>
+      <c r="E50">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>500</v>
+      </c>
+      <c r="C51">
+        <v>50</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.14551999999999998</v>
+      </c>
+      <c r="E51">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>500</v>
+      </c>
+      <c r="C52">
+        <v>125</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.42893599999999998</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>500</v>
+      </c>
+      <c r="C53">
+        <v>250</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.79760829999999994</v>
+      </c>
+      <c r="E53">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>500</v>
+      </c>
+      <c r="C54">
+        <v>25</v>
+      </c>
+      <c r="D54" s="2">
+        <v>7.0008000000000001E-2</v>
+      </c>
+      <c r="E54">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>500</v>
+      </c>
+      <c r="C55">
+        <v>50</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.15113849999999998</v>
+      </c>
+      <c r="E55">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>500</v>
+      </c>
+      <c r="C56">
+        <v>125</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.4153461</v>
+      </c>
+      <c r="E56">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>500</v>
+      </c>
+      <c r="C57">
+        <v>250</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.77092299999999991</v>
+      </c>
+      <c r="E57">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>500</v>
+      </c>
+      <c r="C58">
+        <v>25</v>
+      </c>
+      <c r="D58" s="2">
+        <v>6.7706199999999994E-2</v>
+      </c>
+      <c r="E58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>500</v>
+      </c>
+      <c r="C59">
+        <v>50</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.14233470000000001</v>
+      </c>
+      <c r="E59">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>500</v>
+      </c>
+      <c r="C60">
+        <v>125</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.40409100000000003</v>
+      </c>
+      <c r="E60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>500</v>
+      </c>
+      <c r="C61">
+        <v>250</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.84517300000000006</v>
+      </c>
+      <c r="E61">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>500</v>
+      </c>
+      <c r="C62">
+        <v>25</v>
+      </c>
+      <c r="D62" s="2">
+        <v>7.4250999999999998E-2</v>
+      </c>
+      <c r="E62">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>500</v>
+      </c>
+      <c r="C63">
+        <v>50</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.14752319999999999</v>
+      </c>
+      <c r="E63">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>500</v>
+      </c>
+      <c r="C64">
+        <v>125</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.4178675</v>
+      </c>
+      <c r="E64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>500</v>
+      </c>
+      <c r="C65">
+        <v>250</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.76309979999999999</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>500</v>
+      </c>
+      <c r="C66">
+        <v>25</v>
+      </c>
+      <c r="D66" s="2">
+        <v>7.6448600000000005E-2</v>
+      </c>
+      <c r="E66">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>500</v>
+      </c>
+      <c r="C67">
+        <v>50</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.1539557</v>
+      </c>
+      <c r="E67">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>500</v>
+      </c>
+      <c r="C68">
+        <v>125</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.43411749999999999</v>
+      </c>
+      <c r="E68">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>500</v>
+      </c>
+      <c r="C69">
+        <v>250</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.78429890000000002</v>
+      </c>
+      <c r="E69">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>500</v>
+      </c>
+      <c r="C70">
+        <v>25</v>
+      </c>
+      <c r="D70" s="2">
+        <v>7.8806000000000001E-2</v>
+      </c>
+      <c r="E70">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>500</v>
+      </c>
+      <c r="C71">
+        <v>50</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.14844390000000002</v>
+      </c>
+      <c r="E71">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>500</v>
+      </c>
+      <c r="C72">
+        <v>125</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.4319751</v>
+      </c>
+      <c r="E72">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>500</v>
+      </c>
+      <c r="C73">
+        <v>250</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.79846200000000001</v>
+      </c>
+      <c r="E73">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74">
+        <v>500</v>
+      </c>
+      <c r="C74">
+        <v>25</v>
+      </c>
+      <c r="D74" s="2">
+        <v>7.7362600000000004E-2</v>
+      </c>
+      <c r="E74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>500</v>
+      </c>
+      <c r="C75">
+        <v>50</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.1584805</v>
+      </c>
+      <c r="E75">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>500</v>
+      </c>
+      <c r="C76">
+        <v>125</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.41067990000000004</v>
+      </c>
+      <c r="E76">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>500</v>
+      </c>
+      <c r="C77">
+        <v>250</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.85320170000000006</v>
+      </c>
+      <c r="E77">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>500</v>
+      </c>
+      <c r="C78">
+        <v>25</v>
+      </c>
+      <c r="D78" s="2">
+        <v>7.2952100000000006E-2</v>
+      </c>
+      <c r="E78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>500</v>
+      </c>
+      <c r="C79">
+        <v>50</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.14549409999999999</v>
+      </c>
+      <c r="E79">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>500</v>
+      </c>
+      <c r="C80">
+        <v>125</v>
+      </c>
+      <c r="D80">
+        <v>0.43105150000000003</v>
+      </c>
+      <c r="E80">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:T80">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="500"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="250"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>